<commit_message>
I made the behavior changeable. I expanded the test.
- new attribute color
- docs
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls3/LinkTest.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls3/LinkTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\jdk21-workspace\jxls-project\jxls-poi\src\test\resources\org\jxls3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\2024\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD98C9-67F1-4CD9-B267-BAA7663B67D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC7196C-9E3C-4596-A28C-9D0B3A61305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="2415" windowWidth="18795" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type="2"</t>
+          <t xml:space="preserve"> type="DOCUMENT" color="PINK"</t>
         </r>
         <r>
           <rPr>
@@ -221,20 +221,20 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>B</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>3")</t>
+          <t>B4</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>")</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C342A762-E3E5-4C74-ABC2-66B208A7B16C}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{C342A762-E3E5-4C74-ABC2-66B208A7B16C}">
       <text>
         <r>
           <rPr>
@@ -335,7 +335,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>label</t>
+          <t>label2</t>
         </r>
         <r>
           <rPr>
@@ -353,7 +353,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>B3</t>
+          <t>B4</t>
         </r>
         <r>
           <rPr>
@@ -377,19 +377,18 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>${label}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <t>${label1}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -397,7 +396,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -405,7 +404,7 @@
     <font>
       <sz val="18"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -425,7 +424,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -435,6 +434,14 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -452,7 +459,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,11 +480,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -781,21 +788,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -809,23 +818,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD4B0A-2EDC-43CB-A843-A386E19F012B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="1:2"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>